<commit_message>
Refactor README files across multiple directories to enhance structure and clarity; add detailed overviews and file listings.
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C22AB0A-447E-4D03-9B92-7B0E954AD5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="25600" windowHeight="12710"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Daria Shushkova</t>
   </si>
@@ -117,29 +113,44 @@
     <t xml:space="preserve">Update Sequence Diagram, State Machine Diagram, Use Case Diagram(04.05.25). Add comments, update variables. </t>
   </si>
   <si>
+    <t>Updated Sequence Diagram, State Machine Diagram, Use Case Diagram(Done 03.05.2025). Added comments, update variables(Done 04.05.2025)</t>
+  </si>
+  <si>
     <t>Update Activity Diagram, Internal Block Diagram(04.05.25)</t>
   </si>
   <si>
+    <t>Done 03.05.25</t>
+  </si>
+  <si>
     <t>Update Requirement Diagram, Parametric Diagram.Optimise state machine, add logic for obsiticale avoidance(04.05.25)</t>
   </si>
   <si>
+    <t>Done 04.05.25</t>
+  </si>
+  <si>
     <t>Update Definition Diagram, Package Diagram(04.05.25)</t>
   </si>
   <si>
-    <t>Done 03.05.25</t>
-  </si>
-  <si>
-    <t>Updated Sequence Diagram, State Machine Diagram, Use Case Diagram(Done 03.05.2025). Added comments, update variables(Done 04.05.2025)</t>
-  </si>
-  <si>
-    <t>Done 04.05.25</t>
+    <t>Uncategorized</t>
+  </si>
+  <si>
+    <t>Readme Documentation</t>
+  </si>
+  <si>
+    <t>Done 25.05.25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,19 +162,349 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -171,12 +512,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -192,18 +776,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -461,33 +1095,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I9" sqref="I9:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="30.109375" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="38.109375" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" customWidth="1"/>
-    <col min="8" max="8" width="41.109375" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
-    <col min="10" max="10" width="41.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5363636363636" customWidth="1"/>
+    <col min="2" max="2" width="20.9636363636364" customWidth="1"/>
+    <col min="3" max="3" width="30.1090909090909" customWidth="1"/>
+    <col min="4" max="4" width="53.7818181818182" customWidth="1"/>
+    <col min="5" max="5" width="30.1090909090909" customWidth="1"/>
+    <col min="6" max="6" width="38.1090909090909" customWidth="1"/>
+    <col min="7" max="7" width="36.3363636363636" customWidth="1"/>
+    <col min="8" max="8" width="41.1090909090909" customWidth="1"/>
+    <col min="9" max="9" width="22.6636363636364" customWidth="1"/>
+    <col min="10" max="10" width="41.6636363636364" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.1090909090909" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="4:10">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
@@ -496,18 +1132,18 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
@@ -528,119 +1164,198 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="36.450000000000003" customHeight="1">
-      <c r="A3" s="2">
+    <row r="3" ht="36.45" customHeight="1" spans="1:11">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="57.45" customHeight="1">
-      <c r="A4" s="2">
+    <row r="4" ht="57.45" customHeight="1" spans="1:11">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="99" customHeight="1">
-      <c r="A5" s="2">
+    <row r="5" ht="99" customHeight="1" spans="1:11">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>31</v>
-      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:11">
+      <c r="A6" s="7"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:11">
+      <c r="A7" s="7"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:11">
+      <c r="A8" s="7"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:11">
+      <c r="A9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:11">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:11">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="3:3">
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="K9:K11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>